<commit_message>
docs: change default language of OnlyOffice docs to french
</commit_message>
<xml_diff>
--- a/LaclasseService/Doc/sample.xlsx
+++ b/LaclasseService/Doc/sample.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Page1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -379,74 +379,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface="Arial"/>
         <a:cs typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface="Arial"/>
         <a:cs typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,7 +394,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -480,7 +420,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -569,7 +509,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -606,9 +546,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
+  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>